<commit_message>
Implemented the afficiate system into project
</commit_message>
<xml_diff>
--- a/backend/web/uploads/books.xlsx
+++ b/backend/web/uploads/books.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56A4487-8AA9-414C-B207-0FB54D225AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731B5A3C-08EA-4A14-A424-1448D8E75764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Title</t>
   </si>
@@ -73,10 +73,7 @@
     <t>Charlie Brown</t>
   </si>
   <si>
-    <t>Acc</t>
-  </si>
-  <si>
-    <t>Abn</t>
+    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -108,7 +105,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -131,13 +128,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -444,15 +455,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,8 +476,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -477,10 +491,13 @@
         <v>1925</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -491,10 +508,13 @@
         <v>1949</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -507,8 +527,11 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -521,8 +544,11 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -534,6 +560,9 @@
       </c>
       <c r="D6" t="s">
         <v>16</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>